<commit_message>
Updated on 04-25-2024 at 19:02
</commit_message>
<xml_diff>
--- a/experiment_2/data/br_100.xlsx
+++ b/experiment_2/data/br_100.xlsx
@@ -8,17 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavoquintero/Documents/github/LOVO2024/experiment_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3680C5A-1259-3E40-98B9-4E23F229599C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{291C94CF-D48A-E746-8C4D-9A0EF70DE0FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17400" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-10840" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$P$152:$P$251</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$P$152:$P$251</definedName>
-  </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -4288,12 +4284,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -4323,12 +4325,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4595,8 +4598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A86" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S111" sqref="S111"/>
+    <sheetView tabSelected="1" topLeftCell="A502" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P456" sqref="P456"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -28056,7 +28059,7 @@
       <c r="O456" s="2">
         <v>17.556000000000001</v>
       </c>
-      <c r="P456" s="2">
+      <c r="P456" s="3">
         <v>12.586</v>
       </c>
       <c r="Q456" s="2">
@@ -28109,7 +28112,7 @@
       <c r="O457" s="2">
         <v>17.969000000000001</v>
       </c>
-      <c r="P457" s="2">
+      <c r="P457" s="3">
         <v>13.82</v>
       </c>
       <c r="Q457" s="2">
@@ -28162,7 +28165,7 @@
       <c r="O458" s="2">
         <v>17.504999999999999</v>
       </c>
-      <c r="P458" s="2">
+      <c r="P458" s="3">
         <v>14.478999999999999</v>
       </c>
       <c r="Q458" s="2">
@@ -28215,7 +28218,7 @@
       <c r="O459" s="2">
         <v>13.571</v>
       </c>
-      <c r="P459" s="2">
+      <c r="P459" s="3">
         <v>13.996</v>
       </c>
       <c r="Q459" s="2">
@@ -28268,7 +28271,7 @@
       <c r="O460" s="2">
         <v>9.2279999999999998</v>
       </c>
-      <c r="P460" s="2">
+      <c r="P460" s="3">
         <v>13.032999999999999</v>
       </c>
       <c r="Q460" s="2">
@@ -28321,7 +28324,7 @@
       <c r="O461" s="2">
         <v>5.7590000000000003</v>
       </c>
-      <c r="P461" s="2">
+      <c r="P461" s="3">
         <v>12.757</v>
       </c>
       <c r="Q461" s="2">
@@ -28374,7 +28377,7 @@
       <c r="O462" s="2">
         <v>6.1260000000000003</v>
       </c>
-      <c r="P462" s="2">
+      <c r="P462" s="3">
         <v>12.531000000000001</v>
       </c>
       <c r="Q462" s="2">
@@ -28427,7 +28430,7 @@
       <c r="O463" s="2">
         <v>19.483000000000001</v>
       </c>
-      <c r="P463" s="2">
+      <c r="P463" s="3">
         <v>12.805999999999999</v>
       </c>
       <c r="Q463" s="2">
@@ -28480,7 +28483,7 @@
       <c r="O464" s="2">
         <v>17.783000000000001</v>
       </c>
-      <c r="P464" s="2">
+      <c r="P464" s="3">
         <v>12.779</v>
       </c>
       <c r="Q464" s="2">
@@ -28533,7 +28536,7 @@
       <c r="O465" s="2">
         <v>19.734000000000002</v>
       </c>
-      <c r="P465" s="2">
+      <c r="P465" s="3">
         <v>13.098000000000001</v>
       </c>
       <c r="Q465" s="2">
@@ -28586,7 +28589,7 @@
       <c r="O466" s="2">
         <v>17.152000000000001</v>
       </c>
-      <c r="P466" s="2">
+      <c r="P466" s="3">
         <v>13.609</v>
       </c>
       <c r="Q466" s="2">
@@ -28639,7 +28642,7 @@
       <c r="O467" s="2">
         <v>12.15</v>
       </c>
-      <c r="P467" s="2">
+      <c r="P467" s="3">
         <v>14.026999999999999</v>
       </c>
       <c r="Q467" s="2">
@@ -28692,7 +28695,7 @@
       <c r="O468" s="2">
         <v>8.3740000000000006</v>
       </c>
-      <c r="P468" s="2">
+      <c r="P468" s="3">
         <v>14.4</v>
       </c>
       <c r="Q468" s="2">
@@ -28745,7 +28748,7 @@
       <c r="O469" s="2">
         <v>6.8739999999999997</v>
       </c>
-      <c r="P469" s="2">
+      <c r="P469" s="3">
         <v>14.507</v>
       </c>
       <c r="Q469" s="2">
@@ -28798,7 +28801,7 @@
       <c r="O470" s="2">
         <v>17.686</v>
       </c>
-      <c r="P470" s="2">
+      <c r="P470" s="3">
         <v>14.25</v>
       </c>
       <c r="Q470" s="2">
@@ -28851,7 +28854,7 @@
       <c r="O471" s="2">
         <v>16.065000000000001</v>
       </c>
-      <c r="P471" s="2">
+      <c r="P471" s="3">
         <v>14.005000000000001</v>
       </c>
       <c r="Q471" s="2">
@@ -28904,7 +28907,7 @@
       <c r="O472" s="2">
         <v>16.533999999999999</v>
       </c>
-      <c r="P472" s="2">
+      <c r="P472" s="3">
         <v>13.548</v>
       </c>
       <c r="Q472" s="2">
@@ -28957,7 +28960,7 @@
       <c r="O473" s="2">
         <v>15.35</v>
       </c>
-      <c r="P473" s="2">
+      <c r="P473" s="3">
         <v>13.29</v>
       </c>
       <c r="Q473" s="2">
@@ -29010,7 +29013,7 @@
       <c r="O474" s="2">
         <v>13.603</v>
       </c>
-      <c r="P474" s="2">
+      <c r="P474" s="3">
         <v>13.497999999999999</v>
       </c>
       <c r="Q474" s="2">
@@ -29063,7 +29066,7 @@
       <c r="O475" s="2">
         <v>7.6959999999999997</v>
       </c>
-      <c r="P475" s="2">
+      <c r="P475" s="3">
         <v>13.401</v>
       </c>
       <c r="Q475" s="2">
@@ -29116,7 +29119,7 @@
       <c r="O476" s="2">
         <v>6.2560000000000002</v>
       </c>
-      <c r="P476" s="2">
+      <c r="P476" s="3">
         <v>13.313000000000001</v>
       </c>
       <c r="Q476" s="2">
@@ -29169,7 +29172,7 @@
       <c r="O477" s="2">
         <v>15.423999999999999</v>
       </c>
-      <c r="P477" s="2">
+      <c r="P477" s="3">
         <v>12.99</v>
       </c>
       <c r="Q477" s="2">
@@ -29222,7 +29225,7 @@
       <c r="O478" s="2">
         <v>16.125</v>
       </c>
-      <c r="P478" s="2">
+      <c r="P478" s="3">
         <v>12.997999999999999</v>
       </c>
       <c r="Q478" s="2">
@@ -29275,7 +29278,7 @@
       <c r="O479" s="2">
         <v>9.4139999999999997</v>
       </c>
-      <c r="P479" s="2">
+      <c r="P479" s="3">
         <v>11.981</v>
       </c>
       <c r="Q479" s="2">
@@ -29328,7 +29331,7 @@
       <c r="O480" s="2">
         <v>13.534000000000001</v>
       </c>
-      <c r="P480" s="2">
+      <c r="P480" s="3">
         <v>11.722</v>
       </c>
       <c r="Q480" s="2">
@@ -29381,7 +29384,7 @@
       <c r="O481" s="2">
         <v>14.286</v>
       </c>
-      <c r="P481" s="2">
+      <c r="P481" s="3">
         <v>11.819000000000001</v>
       </c>
       <c r="Q481" s="2">
@@ -29434,7 +29437,7 @@
       <c r="O482" s="2">
         <v>6.0609999999999999</v>
       </c>
-      <c r="P482" s="2">
+      <c r="P482" s="3">
         <v>11.586</v>
       </c>
       <c r="Q482" s="2">
@@ -29487,7 +29490,7 @@
       <c r="O483" s="2">
         <v>5.29</v>
       </c>
-      <c r="P483" s="2">
+      <c r="P483" s="3">
         <v>11.448</v>
       </c>
       <c r="Q483" s="2">
@@ -29540,7 +29543,7 @@
       <c r="O484" s="2">
         <v>14.333</v>
       </c>
-      <c r="P484" s="2">
+      <c r="P484" s="3">
         <v>11.292</v>
       </c>
       <c r="Q484" s="2">
@@ -29593,7 +29596,7 @@
       <c r="O485" s="2">
         <v>14.69</v>
       </c>
-      <c r="P485" s="2">
+      <c r="P485" s="3">
         <v>11.087</v>
       </c>
       <c r="Q485" s="2">
@@ -29646,7 +29649,7 @@
       <c r="O486" s="2">
         <v>13.938000000000001</v>
       </c>
-      <c r="P486" s="2">
+      <c r="P486" s="3">
         <v>11.733000000000001</v>
       </c>
       <c r="Q486" s="2">
@@ -29699,7 +29702,7 @@
       <c r="O487" s="2">
         <v>12.052</v>
       </c>
-      <c r="P487" s="2">
+      <c r="P487" s="3">
         <v>11.521000000000001</v>
       </c>
       <c r="Q487" s="2">
@@ -29752,7 +29755,7 @@
       <c r="O488" s="2">
         <v>12.336</v>
       </c>
-      <c r="P488" s="2">
+      <c r="P488" s="3">
         <v>11.243</v>
       </c>
       <c r="Q488" s="2">
@@ -29805,7 +29808,7 @@
       <c r="O489" s="2">
         <v>5.5830000000000002</v>
       </c>
-      <c r="P489" s="2">
+      <c r="P489" s="3">
         <v>11.173999999999999</v>
       </c>
       <c r="Q489" s="2">
@@ -29858,7 +29861,7 @@
       <c r="O490" s="2">
         <v>4.5650000000000004</v>
       </c>
-      <c r="P490" s="2">
+      <c r="P490" s="3">
         <v>11.071</v>
       </c>
       <c r="Q490" s="2">
@@ -29911,7 +29914,7 @@
       <c r="O491" s="2">
         <v>13.775</v>
       </c>
-      <c r="P491" s="2">
+      <c r="P491" s="3">
         <v>10.991</v>
       </c>
       <c r="Q491" s="2">
@@ -29964,7 +29967,7 @@
       <c r="O492" s="2">
         <v>13.055</v>
       </c>
-      <c r="P492" s="2">
+      <c r="P492" s="3">
         <v>10.757999999999999</v>
       </c>
       <c r="Q492" s="2">
@@ -30017,7 +30020,7 @@
       <c r="O493" s="2">
         <v>11.843</v>
       </c>
-      <c r="P493" s="2">
+      <c r="P493" s="3">
         <v>10.459</v>
       </c>
       <c r="Q493" s="2">
@@ -30070,7 +30073,7 @@
       <c r="O494" s="2">
         <v>10.055</v>
       </c>
-      <c r="P494" s="2">
+      <c r="P494" s="3">
         <v>10.173</v>
       </c>
       <c r="Q494" s="2">
@@ -30123,7 +30126,7 @@
       <c r="O495" s="2">
         <v>10.227</v>
       </c>
-      <c r="P495" s="2">
+      <c r="P495" s="3">
         <v>9.8719999999999999</v>
       </c>
       <c r="Q495" s="2">
@@ -30176,7 +30179,7 @@
       <c r="O496" s="2">
         <v>4.7560000000000002</v>
       </c>
-      <c r="P496" s="2">
+      <c r="P496" s="3">
         <v>9.7539999999999996</v>
       </c>
       <c r="Q496" s="2">
@@ -30229,7 +30232,7 @@
       <c r="O497" s="2">
         <v>4.1289999999999996</v>
       </c>
-      <c r="P497" s="2">
+      <c r="P497" s="3">
         <v>9.6920000000000002</v>
       </c>
       <c r="Q497" s="2">
@@ -30282,7 +30285,7 @@
       <c r="O498" s="2">
         <v>10.733000000000001</v>
       </c>
-      <c r="P498" s="2">
+      <c r="P498" s="3">
         <v>9.2569999999999997</v>
       </c>
       <c r="Q498" s="2">
@@ -30335,7 +30338,7 @@
       <c r="O499" s="2">
         <v>11.583</v>
       </c>
-      <c r="P499" s="2">
+      <c r="P499" s="3">
         <v>9.0470000000000006</v>
       </c>
       <c r="Q499" s="2">
@@ -30388,7 +30391,7 @@
       <c r="O500" s="2">
         <v>11.068</v>
       </c>
-      <c r="P500" s="2">
+      <c r="P500" s="3">
         <v>8.9359999999999999</v>
       </c>
       <c r="Q500" s="2">
@@ -30441,7 +30444,7 @@
       <c r="O501" s="2">
         <v>10.269</v>
       </c>
-      <c r="P501" s="2">
+      <c r="P501" s="3">
         <v>8.9659999999999993</v>
       </c>
       <c r="Q501" s="2">
@@ -30494,7 +30497,7 @@
       <c r="O502" s="2">
         <v>9.6929999999999996</v>
       </c>
-      <c r="P502" s="2">
+      <c r="P502" s="3">
         <v>8.89</v>
       </c>
       <c r="Q502" s="2">
@@ -30547,7 +30550,7 @@
       <c r="O503" s="2">
         <v>4.8120000000000003</v>
       </c>
-      <c r="P503" s="2">
+      <c r="P503" s="3">
         <v>8.8979999999999997</v>
       </c>
       <c r="Q503" s="2">
@@ -30600,7 +30603,7 @@
       <c r="O504" s="2">
         <v>3.65</v>
       </c>
-      <c r="P504" s="2">
+      <c r="P504" s="3">
         <v>8.83</v>
       </c>
       <c r="Q504" s="2">
@@ -30653,7 +30656,7 @@
       <c r="O505" s="2">
         <v>11.670999999999999</v>
       </c>
-      <c r="P505" s="2">
+      <c r="P505" s="3">
         <v>8.9640000000000004</v>
       </c>
       <c r="Q505" s="2">
@@ -30706,7 +30709,7 @@
       <c r="O506" s="2">
         <v>12.266</v>
       </c>
-      <c r="P506" s="2">
+      <c r="P506" s="3">
         <v>9.0609999999999999</v>
       </c>
       <c r="Q506" s="2">
@@ -30759,7 +30762,7 @@
       <c r="O507" s="2">
         <v>11.16</v>
       </c>
-      <c r="P507" s="2">
+      <c r="P507" s="3">
         <v>9.0739999999999998</v>
       </c>
       <c r="Q507" s="2">
@@ -30812,7 +30815,7 @@
       <c r="O508" s="2">
         <v>10.287000000000001</v>
       </c>
-      <c r="P508" s="2">
+      <c r="P508" s="3">
         <v>9.077</v>
       </c>
       <c r="Q508" s="2">
@@ -30865,7 +30868,7 @@
       <c r="O509" s="2">
         <v>8.82</v>
       </c>
-      <c r="P509" s="2">
+      <c r="P509" s="3">
         <v>8.952</v>
       </c>
       <c r="Q509" s="2">
@@ -30918,7 +30921,7 @@
       <c r="O510" s="2">
         <v>3.9940000000000002</v>
       </c>
-      <c r="P510" s="2">
+      <c r="P510" s="3">
         <v>8.8360000000000003</v>
       </c>
       <c r="Q510" s="2">
@@ -30971,7 +30974,7 @@
       <c r="O511" s="2">
         <v>3.669</v>
       </c>
-      <c r="P511" s="2">
+      <c r="P511" s="3">
         <v>8.8379999999999992</v>
       </c>
       <c r="Q511" s="2">
@@ -31024,7 +31027,7 @@
       <c r="O512" s="2">
         <v>10.092000000000001</v>
       </c>
-      <c r="P512" s="2">
+      <c r="P512" s="3">
         <v>8.6129999999999995</v>
       </c>
       <c r="Q512" s="2">
@@ -31077,7 +31080,7 @@
       <c r="O513" s="2">
         <v>11.137</v>
       </c>
-      <c r="P513" s="2">
+      <c r="P513" s="3">
         <v>8.4510000000000005</v>
       </c>
       <c r="Q513" s="2">
@@ -31130,7 +31133,7 @@
       <c r="O514" s="2">
         <v>10.427</v>
       </c>
-      <c r="P514" s="2">
+      <c r="P514" s="3">
         <v>8.3469999999999995</v>
       </c>
       <c r="Q514" s="2">
@@ -31183,7 +31186,7 @@
       <c r="O515" s="2">
         <v>11.012</v>
       </c>
-      <c r="P515" s="2">
+      <c r="P515" s="3">
         <v>8.4499999999999993</v>
       </c>
       <c r="Q515" s="2">
@@ -31236,7 +31239,7 @@
       <c r="O516" s="2">
         <v>9.3450000000000006</v>
       </c>
-      <c r="P516" s="2">
+      <c r="P516" s="3">
         <v>8.5250000000000004</v>
       </c>
       <c r="Q516" s="2">
@@ -31289,7 +31292,7 @@
       <c r="O517" s="2">
         <v>4.0590000000000002</v>
       </c>
-      <c r="P517" s="2">
+      <c r="P517" s="3">
         <v>8.5340000000000007</v>
       </c>
       <c r="Q517" s="2">
@@ -31342,7 +31345,7 @@
       <c r="O518" s="2">
         <v>3.9940000000000002</v>
       </c>
-      <c r="P518" s="2">
+      <c r="P518" s="3">
         <v>8.5809999999999995</v>
       </c>
       <c r="Q518" s="2">
@@ -31395,7 +31398,7 @@
       <c r="O519" s="2">
         <v>11.183999999999999</v>
       </c>
-      <c r="P519" s="2">
+      <c r="P519" s="3">
         <v>8.7370000000000001</v>
       </c>
       <c r="Q519" s="2">
@@ -31448,7 +31451,7 @@
       <c r="O520" s="2">
         <v>11.643000000000001</v>
       </c>
-      <c r="P520" s="2">
+      <c r="P520" s="3">
         <v>8.8089999999999993</v>
       </c>
       <c r="Q520" s="2">
@@ -31501,7 +31504,7 @@
       <c r="O521" s="2">
         <v>7.8120000000000003</v>
       </c>
-      <c r="P521" s="2">
+      <c r="P521" s="3">
         <v>8.4359999999999999</v>
       </c>
       <c r="Q521" s="2">
@@ -31554,7 +31557,7 @@
       <c r="O522" s="2">
         <v>6.7530000000000001</v>
       </c>
-      <c r="P522" s="2">
+      <c r="P522" s="3">
         <v>7.827</v>
       </c>
       <c r="Q522" s="2">
@@ -31607,7 +31610,7 @@
       <c r="O523" s="2">
         <v>7.8440000000000003</v>
       </c>
-      <c r="P523" s="2">
+      <c r="P523" s="3">
         <v>7.6130000000000004</v>
       </c>
       <c r="Q523" s="2">
@@ -31660,7 +31663,7 @@
       <c r="O524" s="2">
         <v>4.0549999999999997</v>
       </c>
-      <c r="P524" s="2">
+      <c r="P524" s="3">
         <v>7.6120000000000001</v>
       </c>
       <c r="Q524" s="2">
@@ -31713,7 +31716,7 @@
       <c r="O525" s="2">
         <v>4.6909999999999998</v>
       </c>
-      <c r="P525" s="2">
+      <c r="P525" s="3">
         <v>7.7119999999999997</v>
       </c>
       <c r="Q525" s="2">
@@ -31766,7 +31769,7 @@
       <c r="O526" s="2">
         <v>11.044</v>
       </c>
-      <c r="P526" s="2">
+      <c r="P526" s="3">
         <v>7.6920000000000002</v>
       </c>
       <c r="Q526" s="2">
@@ -31819,7 +31822,7 @@
       <c r="O527" s="2">
         <v>12.647</v>
       </c>
-      <c r="P527" s="2">
+      <c r="P527" s="3">
         <v>7.835</v>
       </c>
       <c r="Q527" s="2">
@@ -31872,7 +31875,7 @@
       <c r="O528" s="2">
         <v>11.63</v>
       </c>
-      <c r="P528" s="2">
+      <c r="P528" s="3">
         <v>8.3800000000000008</v>
       </c>
       <c r="Q528" s="2">
@@ -31925,7 +31928,7 @@
       <c r="O529" s="2">
         <v>10.292</v>
       </c>
-      <c r="P529" s="2">
+      <c r="P529" s="3">
         <v>8.8859999999999992</v>
       </c>
       <c r="Q529" s="2">
@@ -31978,7 +31981,7 @@
       <c r="O530" s="2">
         <v>9.4610000000000003</v>
       </c>
-      <c r="P530" s="2">
+      <c r="P530" s="3">
         <v>9.1170000000000009</v>
       </c>
       <c r="Q530" s="2">
@@ -32031,7 +32034,7 @@
       <c r="O531" s="2">
         <v>5.2439999999999998</v>
       </c>
-      <c r="P531" s="2">
+      <c r="P531" s="3">
         <v>9.2870000000000008</v>
       </c>
       <c r="Q531" s="2">
@@ -32084,7 +32087,7 @@
       <c r="O532" s="2">
         <v>3.8410000000000002</v>
       </c>
-      <c r="P532" s="2">
+      <c r="P532" s="3">
         <v>9.1649999999999991</v>
       </c>
       <c r="Q532" s="2">
@@ -32137,7 +32140,7 @@
       <c r="O533" s="2">
         <v>11.462</v>
       </c>
-      <c r="P533" s="2">
+      <c r="P533" s="3">
         <v>9.2249999999999996</v>
       </c>
       <c r="Q533" s="2">
@@ -32190,7 +32193,7 @@
       <c r="O534" s="2">
         <v>13.919</v>
       </c>
-      <c r="P534" s="2">
+      <c r="P534" s="3">
         <v>9.407</v>
       </c>
       <c r="Q534" s="2">
@@ -32243,7 +32246,7 @@
       <c r="O535" s="2">
         <v>10.733000000000001</v>
       </c>
-      <c r="P535" s="2">
+      <c r="P535" s="3">
         <v>9.2789999999999999</v>
       </c>
       <c r="Q535" s="2">
@@ -32296,7 +32299,7 @@
       <c r="O536" s="2">
         <v>11.587999999999999</v>
       </c>
-      <c r="P536" s="2">
+      <c r="P536" s="3">
         <v>9.4640000000000004</v>
       </c>
       <c r="Q536" s="2">
@@ -32349,7 +32352,7 @@
       <c r="O537" s="2">
         <v>10.686999999999999</v>
       </c>
-      <c r="P537" s="2">
+      <c r="P537" s="3">
         <v>9.6389999999999993</v>
       </c>
       <c r="Q537" s="2">
@@ -32402,7 +32405,7 @@
       <c r="O538" s="2">
         <v>4.7610000000000001</v>
       </c>
-      <c r="P538" s="2">
+      <c r="P538" s="3">
         <v>9.57</v>
       </c>
       <c r="Q538" s="2">
@@ -32455,7 +32458,7 @@
       <c r="O539" s="2">
         <v>3.5339999999999998</v>
       </c>
-      <c r="P539" s="2">
+      <c r="P539" s="3">
         <v>9.5259999999999998</v>
       </c>
       <c r="Q539" s="2">
@@ -32508,7 +32511,7 @@
       <c r="O540" s="2">
         <v>9.8970000000000002</v>
       </c>
-      <c r="P540" s="2">
+      <c r="P540" s="3">
         <v>9.3030000000000008</v>
       </c>
       <c r="Q540" s="2">
@@ -32561,7 +32564,7 @@
       <c r="O541" s="2">
         <v>11.109</v>
       </c>
-      <c r="P541" s="2">
+      <c r="P541" s="3">
         <v>8.9009999999999998</v>
       </c>
       <c r="Q541" s="2">
@@ -32614,7 +32617,7 @@
       <c r="O542" s="2">
         <v>9.4369999999999994</v>
       </c>
-      <c r="P542" s="2">
+      <c r="P542" s="3">
         <v>8.7159999999999993</v>
       </c>
       <c r="Q542" s="2">
@@ -32667,7 +32670,7 @@
       <c r="O543" s="2">
         <v>9.2929999999999993</v>
       </c>
-      <c r="P543" s="2">
+      <c r="P543" s="3">
         <v>8.3879999999999999</v>
       </c>
       <c r="Q543" s="2">
@@ -32720,7 +32723,7 @@
       <c r="O544" s="2">
         <v>7.399</v>
       </c>
-      <c r="P544" s="2">
+      <c r="P544" s="3">
         <v>7.9189999999999996</v>
       </c>
       <c r="Q544" s="2">
@@ -32773,7 +32776,7 @@
       <c r="O545" s="2">
         <v>3.4319999999999999</v>
       </c>
-      <c r="P545" s="2">
+      <c r="P545" s="3">
         <v>7.7290000000000001</v>
       </c>
       <c r="Q545" s="2">
@@ -32826,7 +32829,7 @@
       <c r="O546" s="2">
         <v>2.87</v>
       </c>
-      <c r="P546" s="2">
+      <c r="P546" s="3">
         <v>7.6340000000000003</v>
       </c>
       <c r="Q546" s="2">
@@ -32879,7 +32882,7 @@
       <c r="O547" s="2">
         <v>8.7919999999999998</v>
       </c>
-      <c r="P547" s="2">
+      <c r="P547" s="3">
         <v>7.476</v>
       </c>
       <c r="Q547" s="2">
@@ -32932,7 +32935,7 @@
       <c r="O548" s="2">
         <v>9.6649999999999991</v>
       </c>
-      <c r="P548" s="2">
+      <c r="P548" s="3">
         <v>7.27</v>
       </c>
       <c r="Q548" s="2">
@@ -32985,7 +32988,7 @@
       <c r="O549" s="2">
         <v>9.423</v>
       </c>
-      <c r="P549" s="2">
+      <c r="P549" s="3">
         <v>7.2679999999999998</v>
       </c>
       <c r="Q549" s="2">
@@ -33038,7 +33041,7 @@
       <c r="O550" s="2">
         <v>8.625</v>
       </c>
-      <c r="P550" s="2">
+      <c r="P550" s="3">
         <v>7.1719999999999997</v>
       </c>
       <c r="Q550" s="2">
@@ -33091,7 +33094,7 @@
       <c r="O551" s="2">
         <v>7.5940000000000003</v>
       </c>
-      <c r="P551" s="2">
+      <c r="P551" s="3">
         <v>7.2</v>
       </c>
       <c r="Q551" s="2">
@@ -33144,7 +33147,7 @@
       <c r="O552" s="2">
         <v>3.855</v>
       </c>
-      <c r="P552" s="2">
+      <c r="P552" s="3">
         <v>7.2610000000000001</v>
       </c>
       <c r="Q552" s="2">
@@ -33197,7 +33200,7 @@
       <c r="O553" s="2">
         <v>3.2280000000000002</v>
       </c>
-      <c r="P553" s="2">
+      <c r="P553" s="3">
         <v>7.3120000000000003</v>
       </c>
       <c r="Q553" s="2">
@@ -33250,7 +33253,7 @@
       <c r="O554" s="2">
         <v>8.2669999999999995</v>
       </c>
-      <c r="P554" s="2">
+      <c r="P554" s="3">
         <v>7.2370000000000001</v>
       </c>
       <c r="Q554" s="2">
@@ -33303,7 +33306,7 @@
       <c r="O555" s="2">
         <v>7.6539999999999999</v>
       </c>
-      <c r="P555" s="2">
+      <c r="P555" s="3">
         <v>6.9489999999999998</v>
       </c>
       <c r="Q555" s="2">

</xml_diff>

<commit_message>
Updated on 05-01-2024 at 10:02
</commit_message>
<xml_diff>
--- a/experiment_2/data/br_100.xlsx
+++ b/experiment_2/data/br_100.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavoquintero/Documents/github/LOVO2024/experiment_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B529D31-68A3-6045-8227-BEB04B389D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7EDEB5-9BA5-5142-9D2A-8D8E02BBDAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-10840" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-9100" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4284,7 +4284,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4300,6 +4300,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4331,13 +4337,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4604,8 +4611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A440" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P481" sqref="P481"/>
+    <sheetView tabSelected="1" topLeftCell="A469" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A531" sqref="A531"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -28992,7 +28999,7 @@
       </c>
     </row>
     <row r="481" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A481" t="s">
+      <c r="A481" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B481" t="s">
@@ -29037,7 +29044,7 @@
       <c r="O481">
         <v>14.286</v>
       </c>
-      <c r="P481" s="2">
+      <c r="P481" s="4">
         <v>11.819000000000001</v>
       </c>
       <c r="Q481">
@@ -29090,7 +29097,7 @@
       <c r="O482">
         <v>6.0609999999999999</v>
       </c>
-      <c r="P482" s="2">
+      <c r="P482" s="4">
         <v>11.586</v>
       </c>
       <c r="Q482">
@@ -29143,7 +29150,7 @@
       <c r="O483">
         <v>5.29</v>
       </c>
-      <c r="P483" s="2">
+      <c r="P483" s="4">
         <v>11.448</v>
       </c>
       <c r="Q483">
@@ -29196,7 +29203,7 @@
       <c r="O484">
         <v>14.333</v>
       </c>
-      <c r="P484" s="2">
+      <c r="P484" s="4">
         <v>11.292</v>
       </c>
       <c r="Q484">
@@ -29249,7 +29256,7 @@
       <c r="O485">
         <v>14.69</v>
       </c>
-      <c r="P485" s="2">
+      <c r="P485" s="4">
         <v>11.087</v>
       </c>
       <c r="Q485">
@@ -30317,7 +30324,7 @@
       </c>
     </row>
     <row r="506" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A506" t="s">
+      <c r="A506" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B506" t="s">
@@ -30362,7 +30369,7 @@
       <c r="O506">
         <v>12.266</v>
       </c>
-      <c r="P506" s="2">
+      <c r="P506" s="4">
         <v>9.0609999999999999</v>
       </c>
       <c r="Q506">
@@ -30415,7 +30422,7 @@
       <c r="O507">
         <v>11.16</v>
       </c>
-      <c r="P507" s="2">
+      <c r="P507" s="4">
         <v>9.0739999999999998</v>
       </c>
       <c r="Q507">
@@ -30468,7 +30475,7 @@
       <c r="O508">
         <v>10.287000000000001</v>
       </c>
-      <c r="P508" s="2">
+      <c r="P508" s="4">
         <v>9.077</v>
       </c>
       <c r="Q508">
@@ -30521,7 +30528,7 @@
       <c r="O509">
         <v>8.82</v>
       </c>
-      <c r="P509" s="2">
+      <c r="P509" s="4">
         <v>8.952</v>
       </c>
       <c r="Q509">
@@ -30574,7 +30581,7 @@
       <c r="O510">
         <v>3.9940000000000002</v>
       </c>
-      <c r="P510" s="2">
+      <c r="P510" s="4">
         <v>8.8360000000000003</v>
       </c>
       <c r="Q510">
@@ -31642,7 +31649,7 @@
       </c>
     </row>
     <row r="531" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A531" t="s">
+      <c r="A531" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B531" t="s">
@@ -31687,7 +31694,7 @@
       <c r="O531">
         <v>5.2439999999999998</v>
       </c>
-      <c r="P531" s="2">
+      <c r="P531" s="4">
         <v>9.2870000000000008</v>
       </c>
       <c r="Q531">
@@ -31740,7 +31747,7 @@
       <c r="O532">
         <v>3.8410000000000002</v>
       </c>
-      <c r="P532" s="2">
+      <c r="P532" s="4">
         <v>9.1649999999999991</v>
       </c>
       <c r="Q532">
@@ -31793,7 +31800,7 @@
       <c r="O533">
         <v>11.462</v>
       </c>
-      <c r="P533" s="2">
+      <c r="P533" s="4">
         <v>9.2249999999999996</v>
       </c>
       <c r="Q533">
@@ -31846,7 +31853,7 @@
       <c r="O534">
         <v>13.919</v>
       </c>
-      <c r="P534" s="2">
+      <c r="P534" s="4">
         <v>9.407</v>
       </c>
       <c r="Q534">
@@ -31899,7 +31906,7 @@
       <c r="O535">
         <v>10.733000000000001</v>
       </c>
-      <c r="P535" s="2">
+      <c r="P535" s="4">
         <v>9.2789999999999999</v>
       </c>
       <c r="Q535">

</xml_diff>

<commit_message>
Updated on 05-02-2024 at 11:11
</commit_message>
<xml_diff>
--- a/experiment_2/data/br_100.xlsx
+++ b/experiment_2/data/br_100.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavoquintero/Documents/github/LOVO2024/experiment_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7EDEB5-9BA5-5142-9D2A-8D8E02BBDAC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA724AF-2351-4945-8A1C-CB21DC8A8B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-9100" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4284,7 +4284,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4306,6 +4306,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4337,7 +4343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -4345,6 +4351,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4611,8 +4618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A469" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A531" sqref="A531"/>
+    <sheetView tabSelected="1" topLeftCell="A444" zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P461" sqref="P461"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27674,7 +27681,7 @@
       </c>
     </row>
     <row r="456" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A456" t="s">
+      <c r="A456" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B456" t="s">
@@ -27939,7 +27946,7 @@
       </c>
     </row>
     <row r="461" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A461" t="s">
+      <c r="A461" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B461" t="s">
@@ -27984,7 +27991,7 @@
       <c r="O461">
         <v>5.7590000000000003</v>
       </c>
-      <c r="P461" s="3">
+      <c r="P461" s="4">
         <v>12.757</v>
       </c>
       <c r="Q461">
@@ -28204,7 +28211,7 @@
       </c>
     </row>
     <row r="466" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A466" t="s">
+      <c r="A466" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B466" t="s">
@@ -28249,7 +28256,7 @@
       <c r="O466">
         <v>17.152000000000001</v>
       </c>
-      <c r="P466" s="3">
+      <c r="P466" s="4">
         <v>13.609</v>
       </c>
       <c r="Q466">
@@ -28469,7 +28476,7 @@
       </c>
     </row>
     <row r="471" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A471" t="s">
+      <c r="A471" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B471" t="s">
@@ -28514,7 +28521,7 @@
       <c r="O471">
         <v>16.065000000000001</v>
       </c>
-      <c r="P471" s="3">
+      <c r="P471" s="4">
         <v>14.005000000000001</v>
       </c>
       <c r="Q471">
@@ -28734,7 +28741,7 @@
       </c>
     </row>
     <row r="476" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A476" t="s">
+      <c r="A476" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B476" t="s">
@@ -28779,7 +28786,7 @@
       <c r="O476">
         <v>6.2560000000000002</v>
       </c>
-      <c r="P476" s="3">
+      <c r="P476" s="4">
         <v>13.313000000000001</v>
       </c>
       <c r="Q476">

</xml_diff>

<commit_message>
Updated on 05-02-2024 at 13:16
</commit_message>
<xml_diff>
--- a/experiment_2/data/br_100.xlsx
+++ b/experiment_2/data/br_100.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavoquintero/Documents/github/LOVO2024/experiment_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BA724AF-2351-4945-8A1C-CB21DC8A8B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC3D647-70B9-C148-BDC1-DDE524439BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-9100" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4343,7 +4343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -4352,6 +4352,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4618,8 +4619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A444" zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P461" sqref="P461"/>
+    <sheetView tabSelected="1" topLeftCell="A463" zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T489" sqref="T489"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27946,7 +27947,7 @@
       </c>
     </row>
     <row r="461" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A461" s="4" t="s">
+      <c r="A461" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B461" t="s">
@@ -27991,7 +27992,7 @@
       <c r="O461">
         <v>5.7590000000000003</v>
       </c>
-      <c r="P461" s="4">
+      <c r="P461" s="3">
         <v>12.757</v>
       </c>
       <c r="Q461">
@@ -28211,7 +28212,7 @@
       </c>
     </row>
     <row r="466" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A466" s="4" t="s">
+      <c r="A466" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B466" t="s">
@@ -28256,7 +28257,7 @@
       <c r="O466">
         <v>17.152000000000001</v>
       </c>
-      <c r="P466" s="4">
+      <c r="P466" s="3">
         <v>13.609</v>
       </c>
       <c r="Q466">
@@ -28476,7 +28477,7 @@
       </c>
     </row>
     <row r="471" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A471" s="4" t="s">
+      <c r="A471" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B471" t="s">
@@ -28521,7 +28522,7 @@
       <c r="O471">
         <v>16.065000000000001</v>
       </c>
-      <c r="P471" s="4">
+      <c r="P471" s="3">
         <v>14.005000000000001</v>
       </c>
       <c r="Q471">
@@ -28741,7 +28742,7 @@
       </c>
     </row>
     <row r="476" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A476" s="4" t="s">
+      <c r="A476" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B476" t="s">
@@ -28786,7 +28787,7 @@
       <c r="O476">
         <v>6.2560000000000002</v>
       </c>
-      <c r="P476" s="4">
+      <c r="P476" s="3">
         <v>13.313000000000001</v>
       </c>
       <c r="Q476">
@@ -29006,7 +29007,7 @@
       </c>
     </row>
     <row r="481" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A481" s="4" t="s">
+      <c r="A481" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B481" t="s">
@@ -30013,7 +30014,7 @@
       </c>
     </row>
     <row r="500" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A500" t="s">
+      <c r="A500" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B500" t="s">
@@ -30058,7 +30059,7 @@
       <c r="O500">
         <v>11.068</v>
       </c>
-      <c r="P500" s="2">
+      <c r="P500" s="4">
         <v>8.9359999999999999</v>
       </c>
       <c r="Q500">
@@ -30331,7 +30332,7 @@
       </c>
     </row>
     <row r="506" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A506" s="4" t="s">
+      <c r="A506" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B506" t="s">
@@ -30376,7 +30377,7 @@
       <c r="O506">
         <v>12.266</v>
       </c>
-      <c r="P506" s="4">
+      <c r="P506" s="2">
         <v>9.0609999999999999</v>
       </c>
       <c r="Q506">
@@ -30429,7 +30430,7 @@
       <c r="O507">
         <v>11.16</v>
       </c>
-      <c r="P507" s="4">
+      <c r="P507" s="2">
         <v>9.0739999999999998</v>
       </c>
       <c r="Q507">
@@ -30482,7 +30483,7 @@
       <c r="O508">
         <v>10.287000000000001</v>
       </c>
-      <c r="P508" s="4">
+      <c r="P508" s="2">
         <v>9.077</v>
       </c>
       <c r="Q508">
@@ -30535,7 +30536,7 @@
       <c r="O509">
         <v>8.82</v>
       </c>
-      <c r="P509" s="4">
+      <c r="P509" s="2">
         <v>8.952</v>
       </c>
       <c r="Q509">
@@ -30588,7 +30589,7 @@
       <c r="O510">
         <v>3.9940000000000002</v>
       </c>
-      <c r="P510" s="4">
+      <c r="P510" s="2">
         <v>8.8360000000000003</v>
       </c>
       <c r="Q510">
@@ -31656,7 +31657,7 @@
       </c>
     </row>
     <row r="531" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A531" s="4" t="s">
+      <c r="A531" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B531" t="s">
@@ -31701,7 +31702,7 @@
       <c r="O531">
         <v>5.2439999999999998</v>
       </c>
-      <c r="P531" s="4">
+      <c r="P531" s="2">
         <v>9.2870000000000008</v>
       </c>
       <c r="Q531">
@@ -31754,7 +31755,7 @@
       <c r="O532">
         <v>3.8410000000000002</v>
       </c>
-      <c r="P532" s="4">
+      <c r="P532" s="2">
         <v>9.1649999999999991</v>
       </c>
       <c r="Q532">
@@ -31807,7 +31808,7 @@
       <c r="O533">
         <v>11.462</v>
       </c>
-      <c r="P533" s="4">
+      <c r="P533" s="2">
         <v>9.2249999999999996</v>
       </c>
       <c r="Q533">
@@ -31860,7 +31861,7 @@
       <c r="O534">
         <v>13.919</v>
       </c>
-      <c r="P534" s="4">
+      <c r="P534" s="2">
         <v>9.407</v>
       </c>
       <c r="Q534">
@@ -31913,7 +31914,7 @@
       <c r="O535">
         <v>10.733000000000001</v>
       </c>
-      <c r="P535" s="4">
+      <c r="P535" s="2">
         <v>9.2789999999999999</v>
       </c>
       <c r="Q535">

</xml_diff>

<commit_message>
Updated on 05-03-2024 at 07:22
</commit_message>
<xml_diff>
--- a/experiment_2/data/br_100.xlsx
+++ b/experiment_2/data/br_100.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gustavoquintero/Documents/github/LOVO2024/experiment_2/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FC3D647-70B9-C148-BDC1-DDE524439BF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36383B58-467A-5742-9A6A-996CAD253117}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38400" yWindow="-9100" windowWidth="38400" windowHeight="21100" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4343,7 +4343,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -4352,7 +4352,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4619,8 +4618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q1393"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A463" zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T489" sqref="T489"/>
+    <sheetView tabSelected="1" topLeftCell="A474" zoomScale="109" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P500" sqref="P500"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -27947,7 +27946,7 @@
       </c>
     </row>
     <row r="461" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A461" s="6" t="s">
+      <c r="A461" t="s">
         <v>17</v>
       </c>
       <c r="B461" t="s">
@@ -28212,7 +28211,7 @@
       </c>
     </row>
     <row r="466" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A466" s="6" t="s">
+      <c r="A466" t="s">
         <v>17</v>
       </c>
       <c r="B466" t="s">
@@ -28477,7 +28476,7 @@
       </c>
     </row>
     <row r="471" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A471" s="6" t="s">
+      <c r="A471" t="s">
         <v>17</v>
       </c>
       <c r="B471" t="s">
@@ -28689,7 +28688,7 @@
       </c>
     </row>
     <row r="475" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A475" t="s">
+      <c r="A475" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B475" t="s">
@@ -28742,7 +28741,7 @@
       </c>
     </row>
     <row r="476" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A476" s="6" t="s">
+      <c r="A476" t="s">
         <v>17</v>
       </c>
       <c r="B476" t="s">
@@ -28954,7 +28953,7 @@
       </c>
     </row>
     <row r="480" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A480" t="s">
+      <c r="A480" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B480" t="s">
@@ -29007,7 +29006,7 @@
       </c>
     </row>
     <row r="481" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A481" s="6" t="s">
+      <c r="A481" t="s">
         <v>17</v>
       </c>
       <c r="B481" t="s">
@@ -29052,7 +29051,7 @@
       <c r="O481">
         <v>14.286</v>
       </c>
-      <c r="P481" s="4">
+      <c r="P481" s="2">
         <v>11.819000000000001</v>
       </c>
       <c r="Q481">
@@ -29105,7 +29104,7 @@
       <c r="O482">
         <v>6.0609999999999999</v>
       </c>
-      <c r="P482" s="4">
+      <c r="P482" s="2">
         <v>11.586</v>
       </c>
       <c r="Q482">
@@ -29158,7 +29157,7 @@
       <c r="O483">
         <v>5.29</v>
       </c>
-      <c r="P483" s="4">
+      <c r="P483" s="2">
         <v>11.448</v>
       </c>
       <c r="Q483">
@@ -29211,7 +29210,7 @@
       <c r="O484">
         <v>14.333</v>
       </c>
-      <c r="P484" s="4">
+      <c r="P484" s="2">
         <v>11.292</v>
       </c>
       <c r="Q484">
@@ -29219,7 +29218,7 @@
       </c>
     </row>
     <row r="485" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A485" t="s">
+      <c r="A485" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B485" t="s">
@@ -29264,7 +29263,7 @@
       <c r="O485">
         <v>14.69</v>
       </c>
-      <c r="P485" s="4">
+      <c r="P485" s="2">
         <v>11.087</v>
       </c>
       <c r="Q485">
@@ -29484,7 +29483,7 @@
       </c>
     </row>
     <row r="490" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A490" t="s">
+      <c r="A490" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B490" t="s">
@@ -29749,7 +29748,7 @@
       </c>
     </row>
     <row r="495" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A495" t="s">
+      <c r="A495" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B495" t="s">
@@ -30332,7 +30331,7 @@
       </c>
     </row>
     <row r="506" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A506" s="6" t="s">
+      <c r="A506" t="s">
         <v>17</v>
       </c>
       <c r="B506" t="s">
@@ -31657,7 +31656,7 @@
       </c>
     </row>
     <row r="531" spans="1:17" x14ac:dyDescent="0.15">
-      <c r="A531" s="6" t="s">
+      <c r="A531" t="s">
         <v>17</v>
       </c>
       <c r="B531" t="s">

</xml_diff>